<commit_message>
Small fix in PS table
- disabling DoubleJet90/100_30...Mass_Min620 
- update OnlyMuons column
</commit_message>
<xml_diff>
--- a/official/L1Menu_Collisions2023_v1_2_0/PrescaleTable/L1Menu_Collisions2023_v1_2_0.xlsx
+++ b/official/L1Menu_Collisions2023_v1_2_0/PrescaleTable/L1Menu_Collisions2023_v1_2_0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menu_Collisions2023_v1_2_0/PrescaleTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/L1MenuRun3_LAAAST/official/L1Menu_Collisions2023_v1_2_0/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025B47B3-4BE9-7840-A75E-DE1CB900EFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209D6B31-67F7-F94F-B095-1C581ECE8F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10660" yWindow="-17400" windowWidth="35700" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="580" windowWidth="28800" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="L1Menu_Collisions2023_v1_2_0_te" sheetId="1" r:id="rId1"/>
@@ -1495,8 +1495,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1511,8 +1511,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1567,8 +1567,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1583,8 +1583,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1805,10 +1805,10 @@
   <dimension ref="A1:AD1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H402" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:X412"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3225,7 +3225,7 @@
       <c r="W19" s="6">
         <v>4400</v>
       </c>
-      <c r="X19" s="6">
+      <c r="X19" s="5">
         <v>4400</v>
       </c>
     </row>
@@ -13585,7 +13585,7 @@
       <c r="W159" s="6">
         <v>0</v>
       </c>
-      <c r="X159" s="6">
+      <c r="X159" s="5">
         <v>0</v>
       </c>
     </row>
@@ -16027,7 +16027,7 @@
       <c r="W192" s="5">
         <v>1</v>
       </c>
-      <c r="X192" s="7">
+      <c r="X192" s="5">
         <v>0</v>
       </c>
     </row>
@@ -18691,7 +18691,7 @@
       <c r="W228" s="8">
         <v>50</v>
       </c>
-      <c r="X228" s="8">
+      <c r="X228" s="5">
         <v>50</v>
       </c>
     </row>
@@ -19135,7 +19135,7 @@
       <c r="W234" s="12">
         <v>0</v>
       </c>
-      <c r="X234" s="12">
+      <c r="X234" s="5">
         <v>0</v>
       </c>
     </row>
@@ -23590,7 +23590,7 @@
         <v>0</v>
       </c>
       <c r="D295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E295" s="5">
         <v>0</v>
@@ -23602,55 +23602,55 @@
         <v>0</v>
       </c>
       <c r="H295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="296" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -23738,7 +23738,7 @@
         <v>0</v>
       </c>
       <c r="D297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E297" s="5">
         <v>0</v>
@@ -23750,55 +23750,55 @@
         <v>0</v>
       </c>
       <c r="H297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X297" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="298" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -24907,7 +24907,7 @@
       <c r="W312" s="16">
         <v>1</v>
       </c>
-      <c r="X312" s="16">
+      <c r="X312" s="5">
         <v>1</v>
       </c>
     </row>
@@ -25055,7 +25055,7 @@
       <c r="W314" s="16">
         <v>1</v>
       </c>
-      <c r="X314" s="16">
+      <c r="X314" s="5">
         <v>1</v>
       </c>
     </row>
@@ -25129,7 +25129,7 @@
       <c r="W315" s="16">
         <v>1</v>
       </c>
-      <c r="X315" s="16">
+      <c r="X315" s="5">
         <v>1</v>
       </c>
     </row>
@@ -25277,7 +25277,7 @@
       <c r="W317" s="16">
         <v>1</v>
       </c>
-      <c r="X317" s="16">
+      <c r="X317" s="5">
         <v>1</v>
       </c>
     </row>
@@ -25425,7 +25425,7 @@
       <c r="W319" s="16">
         <v>1</v>
       </c>
-      <c r="X319" s="16">
+      <c r="X319" s="5">
         <v>1</v>
       </c>
     </row>
@@ -25869,7 +25869,7 @@
       <c r="W325" s="9">
         <v>1</v>
       </c>
-      <c r="X325" s="9">
+      <c r="X325" s="5">
         <v>1</v>
       </c>
     </row>
@@ -26091,7 +26091,7 @@
       <c r="W328" s="9">
         <v>1</v>
       </c>
-      <c r="X328" s="9">
+      <c r="X328" s="5">
         <v>1</v>
       </c>
     </row>
@@ -29495,7 +29495,7 @@
       <c r="W374" s="9">
         <v>17581</v>
       </c>
-      <c r="X374" s="9">
+      <c r="X374" s="5">
         <v>17581</v>
       </c>
     </row>
@@ -29569,7 +29569,7 @@
       <c r="W375" s="10">
         <v>0</v>
       </c>
-      <c r="X375" s="10">
+      <c r="X375" s="5">
         <v>0</v>
       </c>
     </row>
@@ -30309,7 +30309,7 @@
       <c r="W385" s="6">
         <v>2239</v>
       </c>
-      <c r="X385" s="6">
+      <c r="X385" s="5">
         <v>2239</v>
       </c>
     </row>
@@ -30383,7 +30383,7 @@
       <c r="W386" s="10">
         <v>1</v>
       </c>
-      <c r="X386" s="10">
+      <c r="X386" s="5">
         <v>1</v>
       </c>
     </row>
@@ -30457,7 +30457,7 @@
       <c r="W387" s="9">
         <v>0</v>
       </c>
-      <c r="X387" s="10">
+      <c r="X387" s="5">
         <v>0</v>
       </c>
     </row>
@@ -30531,7 +30531,7 @@
       <c r="W388" s="9">
         <v>0</v>
       </c>
-      <c r="X388" s="10">
+      <c r="X388" s="5">
         <v>0</v>
       </c>
     </row>
@@ -30605,7 +30605,7 @@
       <c r="W389" s="9">
         <v>0</v>
       </c>
-      <c r="X389" s="10">
+      <c r="X389" s="5">
         <v>0</v>
       </c>
     </row>
@@ -30679,7 +30679,7 @@
       <c r="W390" s="9">
         <v>0</v>
       </c>
-      <c r="X390" s="10">
+      <c r="X390" s="5">
         <v>0</v>
       </c>
     </row>
@@ -30753,7 +30753,7 @@
       <c r="W391" s="6">
         <v>56237</v>
       </c>
-      <c r="X391" s="6">
+      <c r="X391" s="5">
         <v>56237</v>
       </c>
     </row>
@@ -30827,7 +30827,7 @@
       <c r="W392" s="6">
         <v>56237</v>
       </c>
-      <c r="X392" s="6">
+      <c r="X392" s="5">
         <v>56237</v>
       </c>
     </row>
@@ -30901,7 +30901,7 @@
       <c r="W393" s="6">
         <v>59051</v>
       </c>
-      <c r="X393" s="6">
+      <c r="X393" s="5">
         <v>59051</v>
       </c>
     </row>
@@ -30975,7 +30975,7 @@
       <c r="W394" s="5">
         <v>563</v>
       </c>
-      <c r="X394" s="11">
+      <c r="X394" s="5">
         <v>563</v>
       </c>
     </row>
@@ -31863,7 +31863,7 @@
       <c r="W406" s="7">
         <v>3</v>
       </c>
-      <c r="X406" s="7">
+      <c r="X406" s="5">
         <v>3</v>
       </c>
     </row>
@@ -46544,47 +46544,47 @@
       <c r="X1005" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:X167 D168:X233 C168:C295 D235:X295 C296:X296">
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
+  <conditionalFormatting sqref="C2:W167 D168:W233 C168:C295 D235:W295">
+    <cfRule type="cellIs" dxfId="11" priority="21" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C297:X297 C299:X299 C301:X311 C316:X316 C318:X318 C320:X412 C313:X313">
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
+  <conditionalFormatting sqref="C296:W311">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C298:X298">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+  <conditionalFormatting sqref="C313:W313 C316:W316 C318:W318 C320:W412">
+    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="18" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C300:X300">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="X2:X412">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>